<commit_message>
start AD Vina & edited files
</commit_message>
<xml_diff>
--- a/data/task/results/alpha-amylase.xlsx
+++ b/data/task/results/alpha-amylase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\github\bioinformatics\autodock4\data\task\a-glyukoza\result\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\github\bioinformatics\autodock4\data\task\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -225,7 +225,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="uz-Latn-UZ"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1097,7 +1097,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="uz-Latn-UZ"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="379181064"/>
@@ -1156,7 +1156,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="uz-Latn-UZ"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="379173848"/>
@@ -1199,7 +1199,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="uz-Latn-UZ"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1229,7 +1229,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="uz-Latn-UZ"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2083,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I11"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>